<commit_message>
Updated wireframes for Message count
</commit_message>
<xml_diff>
--- a/wireframes/Example Database Search.xlsx
+++ b/wireframes/Example Database Search.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/389717b1d175df99/Development/Projects/ADS-B-BaseStationReader/wireframes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{D66D2F21-3975-4489-8753-E5AC51D47DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C13C524B-8C72-4BA3-A991-96569E6339E8}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{D66D2F21-3975-4489-8753-E5AC51D47DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D895C6D-148B-4298-9BBA-5D48E0C4EA10}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{5E95568F-2D46-475A-8BA4-C753FD79B547}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>Address</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Locked</t>
+  </si>
+  <si>
+    <t>Messages</t>
   </si>
 </sst>
 </file>
@@ -244,6 +247,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -543,11 +550,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D10321-FDF3-4C8C-9A95-4BEC0161FF4E}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -555,10 +560,10 @@
     <col min="2" max="9" width="9.06640625" style="6"/>
     <col min="10" max="10" width="17.86328125" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.86328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.06640625" style="6"/>
+    <col min="12" max="13" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -595,8 +600,11 @@
       <c r="L1" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -633,8 +641,12 @@
       <c r="L2" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M2" s="6">
+        <f ca="1">INT(RAND()*10 + 1.5)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -671,8 +683,12 @@
       <c r="L3" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M3" s="6">
+        <f t="shared" ref="M3:M15" ca="1" si="0">INT(RAND()*10 + 1.5)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -709,8 +725,12 @@
       <c r="L4" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M4" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
@@ -747,8 +767,12 @@
       <c r="L5" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M5" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -785,8 +809,12 @@
       <c r="L6" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M6" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -823,8 +851,12 @@
       <c r="L7" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M7" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>398567</v>
       </c>
@@ -861,8 +893,12 @@
       <c r="L8" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M8" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
@@ -881,8 +917,12 @@
       <c r="L9" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M9" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
@@ -919,8 +959,12 @@
       <c r="L10" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M10" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
@@ -957,8 +1001,12 @@
       <c r="L11" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M11" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
@@ -995,8 +1043,12 @@
       <c r="L12" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M12" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>22</v>
       </c>
@@ -1033,8 +1085,12 @@
       <c r="L13" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M13" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
@@ -1062,8 +1118,12 @@
       <c r="L14" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M14" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
@@ -1099,6 +1159,10 @@
       </c>
       <c r="L15" s="6" t="s">
         <v>38</v>
+      </c>
+      <c r="M15" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added aircraft distance to wireframes
</commit_message>
<xml_diff>
--- a/wireframes/Example Database Search.xlsx
+++ b/wireframes/Example Database Search.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/389717b1d175df99/Development/Projects/ADS-B-BaseStationReader/wireframes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\BaseStationReader\wireframes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{D66D2F21-3975-4489-8753-E5AC51D47DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D895C6D-148B-4298-9BBA-5D48E0C4EA10}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBC89C6-7875-4211-937F-1ABEB6CF9B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{5E95568F-2D46-475A-8BA4-C753FD79B547}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Address</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Messages</t>
+  </si>
+  <si>
+    <t>Distance</t>
   </si>
 </sst>
 </file>
@@ -247,10 +250,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -550,20 +549,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D10321-FDF3-4C8C-9A95-4BEC0161FF4E}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="8.06640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="9.06640625" style="6"/>
-    <col min="10" max="10" width="17.86328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.86328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.06640625" style="6"/>
+    <col min="2" max="10" width="9.06640625" style="6"/>
+    <col min="11" max="11" width="17.86328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -592,19 +591,22 @@
         <v>34</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -632,21 +634,25 @@
       <c r="I2" s="6">
         <v>1280</v>
       </c>
-      <c r="J2" s="7">
-        <v>45184.356574074074</v>
+      <c r="J2" s="6">
+        <f ca="1">INT(RAND()*70 +1.5)</f>
+        <v>20</v>
       </c>
       <c r="K2" s="7">
+        <v>45184.356574074074</v>
+      </c>
+      <c r="L2" s="7">
         <v>45184.356938923615</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="6">
+      <c r="N2" s="6">
         <f ca="1">INT(RAND()*10 + 1.5)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -674,21 +680,25 @@
       <c r="I3" s="6">
         <v>0</v>
       </c>
-      <c r="J3" s="7">
-        <v>45184.356574074074</v>
+      <c r="J3" s="6">
+        <f t="shared" ref="J3:J15" ca="1" si="0">INT(RAND()*70 +1.5)</f>
+        <v>31</v>
       </c>
       <c r="K3" s="7">
+        <v>45184.356574074074</v>
+      </c>
+      <c r="L3" s="7">
         <v>45184.357048611113</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="6">
-        <f t="shared" ref="M3:M15" ca="1" si="0">INT(RAND()*10 + 1.5)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N3" s="6">
+        <f t="shared" ref="N3:N15" ca="1" si="1">INT(RAND()*10 + 1.5)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -716,21 +726,25 @@
       <c r="I4" s="6">
         <v>0</v>
       </c>
-      <c r="J4" s="7">
-        <v>45184.356574074074</v>
+      <c r="J4" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>31</v>
       </c>
       <c r="K4" s="7">
+        <v>45184.356574074074</v>
+      </c>
+      <c r="L4" s="7">
         <v>45184.357074178239</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="M4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N4" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
@@ -758,21 +772,25 @@
       <c r="I5" s="6">
         <v>-768</v>
       </c>
-      <c r="J5" s="7">
-        <v>45184.356574074074</v>
+      <c r="J5" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>31</v>
       </c>
       <c r="K5" s="7">
+        <v>45184.356574074074</v>
+      </c>
+      <c r="L5" s="7">
         <v>45184.357073576386</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="M5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M5" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N5" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -800,21 +818,25 @@
       <c r="I6" s="6">
         <v>1600</v>
       </c>
-      <c r="J6" s="7">
-        <v>45184.356574074074</v>
+      <c r="J6" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
       </c>
       <c r="K6" s="7">
+        <v>45184.356574074074</v>
+      </c>
+      <c r="L6" s="7">
         <v>45184.35707421296</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="M6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N6" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -842,21 +864,25 @@
       <c r="I7" s="6">
         <v>1024</v>
       </c>
-      <c r="J7" s="7">
-        <v>45184.356574074074</v>
+      <c r="J7" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>41</v>
       </c>
       <c r="K7" s="7">
+        <v>45184.356574074074</v>
+      </c>
+      <c r="L7" s="7">
         <v>45184.357074178239</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="M7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M7" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N7" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>398567</v>
       </c>
@@ -884,21 +910,25 @@
       <c r="I8" s="6">
         <v>-2816</v>
       </c>
-      <c r="J8" s="7">
-        <v>45184.356574074074</v>
+      <c r="J8" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>69</v>
       </c>
       <c r="K8" s="7">
+        <v>45184.356574074074</v>
+      </c>
+      <c r="L8" s="7">
         <v>45184.357072951389</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="M8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M8" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N8" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
@@ -908,222 +938,246 @@
       <c r="D9" s="6">
         <v>36000</v>
       </c>
-      <c r="J9" s="7">
-        <v>45184.356574074074</v>
+      <c r="J9" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
       </c>
       <c r="K9" s="7">
+        <v>45184.356574074074</v>
+      </c>
+      <c r="L9" s="7">
         <v>45184.356886574074</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="M9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M9" s="6">
+      <c r="N9" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6">
+        <v>121</v>
+      </c>
+      <c r="D10" s="6">
+        <v>21575</v>
+      </c>
+      <c r="E10" s="6">
+        <v>335</v>
+      </c>
+      <c r="F10" s="6">
+        <v>284</v>
+      </c>
+      <c r="G10" s="6">
+        <v>51.546689999999998</v>
+      </c>
+      <c r="H10" s="6">
+        <v>-1.30653</v>
+      </c>
+      <c r="I10" s="6">
+        <v>-2112</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="K10" s="7">
+        <v>45184.356574074074</v>
+      </c>
+      <c r="L10" s="7">
+        <v>45184.357069791666</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N10" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="6">
+        <v>537</v>
+      </c>
+      <c r="D11" s="6">
+        <v>16225</v>
+      </c>
+      <c r="E11" s="6">
+        <v>364</v>
+      </c>
+      <c r="F11" s="6">
+        <v>217</v>
+      </c>
+      <c r="G11" s="6">
+        <v>51.705849999999998</v>
+      </c>
+      <c r="H11" s="6">
+        <v>-0.49643999999999999</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1856</v>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="K11" s="7">
+        <v>45184.356574074074</v>
+      </c>
+      <c r="L11" s="7">
+        <v>45184.356921296298</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N11" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="6">
+        <v>6346</v>
+      </c>
+      <c r="D12" s="6">
+        <v>36000</v>
+      </c>
+      <c r="E12" s="6">
+        <v>472</v>
+      </c>
+      <c r="F12" s="6">
+        <v>120</v>
+      </c>
+      <c r="G12" s="6">
+        <v>51.705959999999997</v>
+      </c>
+      <c r="H12" s="6">
+        <v>-2.40326</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="K12" s="7">
+        <v>45184.356574074074</v>
+      </c>
+      <c r="L12" s="7">
+        <v>45184.357074201391</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N12" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="6">
+        <v>7342</v>
+      </c>
+      <c r="D13" s="6">
+        <v>9025</v>
+      </c>
+      <c r="E13" s="6">
+        <v>247</v>
+      </c>
+      <c r="F13" s="6">
+        <v>255</v>
+      </c>
+      <c r="G13" s="6">
+        <v>51.607640000000004</v>
+      </c>
+      <c r="H13" s="6">
+        <v>-2.1630400000000001</v>
+      </c>
+      <c r="I13" s="6">
+        <v>-1984</v>
+      </c>
+      <c r="J13" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="K13" s="7">
+        <v>45184.356574074074</v>
+      </c>
+      <c r="L13" s="7">
+        <v>45184.357068506943</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N13" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="6">
+        <v>515</v>
+      </c>
+      <c r="D14" s="6">
+        <v>35025</v>
+      </c>
+      <c r="G14" s="6">
+        <v>51.514890000000001</v>
+      </c>
+      <c r="H14" s="6">
+        <v>-2.8376000000000001</v>
+      </c>
+      <c r="J14" s="6">
         <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="6">
-        <v>121</v>
-      </c>
-      <c r="D10" s="6">
-        <v>21575</v>
-      </c>
-      <c r="E10" s="6">
-        <v>335</v>
-      </c>
-      <c r="F10" s="6">
-        <v>284</v>
-      </c>
-      <c r="G10" s="6">
-        <v>51.546689999999998</v>
-      </c>
-      <c r="H10" s="6">
-        <v>-1.30653</v>
-      </c>
-      <c r="I10" s="6">
-        <v>-2112</v>
-      </c>
-      <c r="J10" s="7">
-        <v>45184.356574074074</v>
-      </c>
-      <c r="K10" s="7">
-        <v>45184.357069791666</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M10" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="6">
-        <v>537</v>
-      </c>
-      <c r="D11" s="6">
-        <v>16225</v>
-      </c>
-      <c r="E11" s="6">
-        <v>364</v>
-      </c>
-      <c r="F11" s="6">
-        <v>217</v>
-      </c>
-      <c r="G11" s="6">
-        <v>51.705849999999998</v>
-      </c>
-      <c r="H11" s="6">
-        <v>-0.49643999999999999</v>
-      </c>
-      <c r="I11" s="6">
-        <v>1856</v>
-      </c>
-      <c r="J11" s="7">
-        <v>45184.356574074074</v>
-      </c>
-      <c r="K11" s="7">
-        <v>45184.356921296298</v>
-      </c>
-      <c r="L11" s="6" t="s">
+      <c r="K14" s="7">
+        <v>45184.356574074074</v>
+      </c>
+      <c r="L14" s="7">
+        <v>45184.356608796297</v>
+      </c>
+      <c r="M14" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M11" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="6">
-        <v>6346</v>
-      </c>
-      <c r="D12" s="6">
-        <v>36000</v>
-      </c>
-      <c r="E12" s="6">
-        <v>472</v>
-      </c>
-      <c r="F12" s="6">
-        <v>120</v>
-      </c>
-      <c r="G12" s="6">
-        <v>51.705959999999997</v>
-      </c>
-      <c r="H12" s="6">
-        <v>-2.40326</v>
-      </c>
-      <c r="I12" s="6">
-        <v>0</v>
-      </c>
-      <c r="J12" s="7">
-        <v>45184.356574074074</v>
-      </c>
-      <c r="K12" s="7">
-        <v>45184.357074201391</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="M12" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="6">
-        <v>7342</v>
-      </c>
-      <c r="D13" s="6">
-        <v>9025</v>
-      </c>
-      <c r="E13" s="6">
-        <v>247</v>
-      </c>
-      <c r="F13" s="6">
-        <v>255</v>
-      </c>
-      <c r="G13" s="6">
-        <v>51.607640000000004</v>
-      </c>
-      <c r="H13" s="6">
-        <v>-2.1630400000000001</v>
-      </c>
-      <c r="I13" s="6">
-        <v>-1984</v>
-      </c>
-      <c r="J13" s="7">
-        <v>45184.356574074074</v>
-      </c>
-      <c r="K13" s="7">
-        <v>45184.357068506943</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="M13" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="6">
-        <v>515</v>
-      </c>
-      <c r="D14" s="6">
-        <v>35025</v>
-      </c>
-      <c r="G14" s="6">
-        <v>51.514890000000001</v>
-      </c>
-      <c r="H14" s="6">
-        <v>-2.8376000000000001</v>
-      </c>
-      <c r="J14" s="7">
-        <v>45184.356574074074</v>
-      </c>
-      <c r="K14" s="7">
-        <v>45184.356608796297</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="M14" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N14" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
@@ -1151,18 +1205,22 @@
       <c r="I15" s="6">
         <v>1472</v>
       </c>
-      <c r="J15" s="7">
-        <v>45184.356574074074</v>
+      <c r="J15" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>69</v>
       </c>
       <c r="K15" s="7">
+        <v>45184.356574074074</v>
+      </c>
+      <c r="L15" s="7">
         <v>45184.357068541663</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="M15" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M15" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+      <c r="N15" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>